<commit_message>
Redo PFLsum1 norms with overlapping age strata with PFLsum2
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/pflsum1-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/pflsum1-raw-ss-lookup-tabbed-age.xlsx
@@ -17,6 +17,12 @@
     <sheet name="8.6-8.11" sheetId="8" r:id="rId8"/>
     <sheet name="9.0-9.5" sheetId="9" r:id="rId9"/>
     <sheet name="9.6-9.11" sheetId="10" r:id="rId10"/>
+    <sheet name="10.0-10.5" sheetId="11" r:id="rId11"/>
+    <sheet name="10.6-10.11" sheetId="12" r:id="rId12"/>
+    <sheet name="11.0-11.5" sheetId="13" r:id="rId13"/>
+    <sheet name="11.6-11.11" sheetId="14" r:id="rId14"/>
+    <sheet name="12.0-12.5" sheetId="15" r:id="rId15"/>
+    <sheet name="12.6-12.11" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -383,7 +389,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
@@ -391,7 +397,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
@@ -399,7 +405,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
@@ -407,7 +413,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
@@ -415,7 +421,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
@@ -423,7 +429,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
@@ -431,7 +437,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
@@ -439,7 +445,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10">
@@ -447,7 +453,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -455,7 +461,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
@@ -463,7 +469,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13">
@@ -471,7 +477,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
@@ -479,7 +485,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15">
@@ -487,7 +493,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16">
@@ -495,7 +501,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17">
@@ -503,7 +509,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18">
@@ -511,7 +517,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19">
@@ -519,7 +525,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20">
@@ -527,7 +533,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
@@ -920,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -928,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
@@ -936,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -944,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -952,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
@@ -960,7 +966,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -968,7 +974,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9">
@@ -976,7 +982,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10">
@@ -984,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
@@ -1040,7 +1046,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18">
@@ -1048,7 +1054,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -1072,7 +1078,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
@@ -1104,7 +1110,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
@@ -1161,6 +1167,3228 @@
       </c>
       <c r="B32">
         <v>129</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>130</v>
       </c>
     </row>
     <row r="33">
@@ -1457,7 +4685,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
@@ -1465,7 +4693,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
@@ -1473,7 +4701,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5">
@@ -1481,7 +4709,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6">
@@ -1489,7 +4717,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7">
@@ -1497,7 +4725,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -1505,7 +4733,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
@@ -1513,7 +4741,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
@@ -1521,7 +4749,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
@@ -1529,7 +4757,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -1537,7 +4765,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13">
@@ -1545,7 +4773,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14">
@@ -1553,7 +4781,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15">
@@ -1561,7 +4789,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16">
@@ -1569,7 +4797,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17">
@@ -1577,7 +4805,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18">
@@ -1585,7 +4813,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19">
@@ -1593,7 +4821,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20">
@@ -1601,7 +4829,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21">
@@ -1609,7 +4837,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22">
@@ -1994,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
@@ -2002,7 +5230,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4">
@@ -2010,7 +5238,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
@@ -2018,7 +5246,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6">
@@ -2026,7 +5254,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
@@ -2034,7 +5262,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
@@ -2042,7 +5270,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
@@ -2050,7 +5278,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
@@ -2058,7 +5286,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11">
@@ -2066,7 +5294,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12">
@@ -2074,7 +5302,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13">
@@ -2082,7 +5310,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14">
@@ -2090,7 +5318,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15">
@@ -2098,7 +5326,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
@@ -2106,7 +5334,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17">
@@ -2114,7 +5342,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18">
@@ -2122,7 +5350,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19">
@@ -2130,7 +5358,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20">
@@ -2138,7 +5366,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21">
@@ -2146,7 +5374,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22">
@@ -2154,7 +5382,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23">
@@ -2563,7 +5791,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
@@ -2571,7 +5799,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8">
@@ -2579,7 +5807,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9">
@@ -2595,7 +5823,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
@@ -2603,7 +5831,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12">
@@ -2611,7 +5839,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
@@ -2627,7 +5855,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15">
@@ -2635,7 +5863,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16">
@@ -2659,7 +5887,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
@@ -2667,7 +5895,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20">
@@ -2691,7 +5919,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23">
@@ -2699,7 +5927,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24">
@@ -3068,7 +6296,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -3132,7 +6360,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11">
@@ -3164,7 +6392,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15">
@@ -3605,7 +6833,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
@@ -3613,7 +6841,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -3621,7 +6849,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -3629,7 +6857,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
@@ -3661,7 +6889,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
@@ -3725,7 +6953,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18">
@@ -3749,7 +6977,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21">
@@ -3757,7 +6985,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22">
@@ -3781,7 +7009,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25">
@@ -3789,7 +7017,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26">
@@ -4142,7 +7370,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
@@ -4150,7 +7378,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
@@ -4158,7 +7386,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
@@ -4166,7 +7394,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
@@ -4174,7 +7402,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
@@ -4182,7 +7410,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8">
@@ -4190,7 +7418,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9">
@@ -4254,7 +7482,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17">
@@ -4262,7 +7490,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18">
@@ -4286,7 +7514,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
@@ -4294,7 +7522,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22">
@@ -4310,7 +7538,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24">
@@ -4318,7 +7546,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25">
@@ -4326,7 +7554,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26">
@@ -4342,7 +7570,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28">
@@ -4679,7 +7907,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
@@ -4687,7 +7915,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -4695,7 +7923,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
@@ -4703,7 +7931,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -4711,7 +7939,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7">
@@ -4719,7 +7947,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
@@ -4727,7 +7955,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
@@ -4735,7 +7963,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
@@ -4759,7 +7987,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
@@ -4767,7 +7995,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
@@ -4799,7 +8027,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18">
@@ -4823,7 +8051,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
@@ -4831,7 +8059,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -4855,7 +8083,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25">
@@ -4863,7 +8091,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26">
@@ -4879,7 +8107,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28">
@@ -4887,7 +8115,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">
@@ -4895,7 +8123,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">
@@ -5216,7 +8444,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -5224,7 +8452,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -5232,7 +8460,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -5240,7 +8468,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -5248,7 +8476,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -5256,7 +8484,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8">
@@ -5264,7 +8492,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
@@ -5272,7 +8500,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
@@ -5344,7 +8572,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -5400,7 +8628,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
@@ -5432,7 +8660,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30">
@@ -5440,7 +8668,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">

</xml_diff>